<commit_message>
Minor code changes. Added document #2
Added document that compares computation time of the different algorithms
</commit_message>
<xml_diff>
--- a/Data_SurfaceRecon.xlsx
+++ b/Data_SurfaceRecon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MicroTomography\MicroTomography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F805302-81C9-4407-948B-C822C2586C82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3AD6C8-77B9-42FE-93D7-E385BED6E2F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{F66D45AC-35CA-471F-BB36-CA15FEE04A93}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="42">
   <si>
     <t>DataPoints:</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t xml:space="preserve">Conclusion : </t>
-  </si>
-  <si>
-    <t>Depending on datasize Norm_Radius and Norm_NN needs to be higher, Norm_Radius can be lower than Norm_NN altough doesn't need to be, but theres no need in it beeing bigger.</t>
   </si>
   <si>
     <t>Ps. Specifically for poisson surface</t>
@@ -171,6 +168,12 @@
       </rPr>
       <t xml:space="preserve"> in this document</t>
     </r>
+  </si>
+  <si>
+    <t>Depending on datasize, Norm_Radius and Norm_NN needs to be higher, Norm_Radius can be lower than Norm_NN altough doesn't need to be, but theres no need in it beeing bigger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norm_Radius and Norm_NN are used to estimate the norms. Basically it searches in the radius for a max of Norm_NN points then uses these to estimate the norm of a point. </t>
   </si>
 </sst>
 </file>
@@ -536,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2A66BA-029E-4727-9F7A-DE9D6FB1A7C5}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,12 +958,17 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -970,7 +978,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1439,7 +1447,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>